<commit_message>
paper add a table
</commit_message>
<xml_diff>
--- a/rulelearning/结果.xlsx
+++ b/rulelearning/结果.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA8C2AC-4A2E-4388-B12C-3A4DD6F35821}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CE9D96-53A2-4C56-A358-E9CD37C8B2F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="89">
   <si>
     <t>Entities</t>
   </si>
@@ -501,6 +501,10 @@
   </si>
   <si>
     <t>5h limit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实体数量不太对！</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1365,7 +1369,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1654,92 +1658,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
@@ -1751,9 +1677,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1794,56 +1717,158 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -2163,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J79" sqref="J79"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2222,13 +2247,13 @@
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="177">
         <v>11024066</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="176">
         <v>3102999</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="177">
         <v>650</v>
       </c>
       <c r="E2" s="12"/>
@@ -2254,13 +2279,13 @@
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="177">
         <v>8397936</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="176">
         <v>3085248</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="177">
         <v>430</v>
       </c>
       <c r="E3" s="12"/>
@@ -2277,13 +2302,13 @@
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="177">
         <v>4125967</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="176">
         <v>2260672</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="177">
         <v>37</v>
       </c>
       <c r="E4" s="12"/>
@@ -2320,16 +2345,16 @@
       <c r="M5" s="11"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="162" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="105">
+      <c r="C6" s="156">
         <v>14951</v>
       </c>
-      <c r="D6" s="105">
+      <c r="D6" s="156">
         <v>1345</v>
       </c>
       <c r="E6" s="18"/>
@@ -2338,7 +2363,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
       <c r="J6" s="28"/>
-      <c r="K6" s="114" t="s">
+      <c r="K6" s="165" t="s">
         <v>6</v>
       </c>
       <c r="L6" s="15" t="s">
@@ -2347,17 +2372,17 @@
       <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="109"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
+      <c r="A7" s="160"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="157"/>
       <c r="E7" s="18"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="28"/>
-      <c r="K7" s="115"/>
+      <c r="K7" s="166"/>
       <c r="L7" s="11" t="s">
         <v>16</v>
       </c>
@@ -2366,17 +2391,17 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="110"/>
-      <c r="B8" s="113"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
+      <c r="A8" s="161"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="158"/>
+      <c r="D8" s="158"/>
       <c r="E8" s="18"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="28"/>
-      <c r="K8" s="116"/>
+      <c r="K8" s="167"/>
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
@@ -2452,7 +2477,7 @@
       <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="120" t="s">
+      <c r="A12" s="150" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="14">
@@ -2475,7 +2500,7 @@
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="121"/>
+      <c r="A13" s="151"/>
       <c r="B13" s="17">
         <v>241158</v>
       </c>
@@ -2496,7 +2521,7 @@
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="120" t="s">
+      <c r="A14" s="150" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="14">
@@ -2519,7 +2544,7 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="121"/>
+      <c r="A15" s="151"/>
       <c r="B15" s="17">
         <v>175412</v>
       </c>
@@ -2539,10 +2564,12 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="175" t="s">
+        <v>88</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -2558,55 +2585,55 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="153" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="122"/>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="122"/>
-      <c r="H18" s="122"/>
-      <c r="I18" s="122"/>
-      <c r="J18" s="122"/>
-      <c r="K18" s="122"/>
-      <c r="L18" s="122"/>
-      <c r="M18" s="122"/>
+      <c r="B18" s="153"/>
+      <c r="C18" s="153"/>
+      <c r="D18" s="153"/>
+      <c r="E18" s="153"/>
+      <c r="F18" s="153"/>
+      <c r="G18" s="153"/>
+      <c r="H18" s="153"/>
+      <c r="I18" s="153"/>
+      <c r="J18" s="153"/>
+      <c r="K18" s="153"/>
+      <c r="L18" s="153"/>
+      <c r="M18" s="153"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="100" t="s">
+      <c r="A19" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="100"/>
-      <c r="I19" s="100"/>
-      <c r="J19" s="100"/>
-      <c r="K19" s="100"/>
-      <c r="L19" s="100"/>
-      <c r="M19" s="100"/>
+      <c r="B19" s="152"/>
+      <c r="C19" s="152"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="152"/>
+      <c r="F19" s="152"/>
+      <c r="G19" s="152"/>
+      <c r="H19" s="152"/>
+      <c r="I19" s="152"/>
+      <c r="J19" s="152"/>
+      <c r="K19" s="152"/>
+      <c r="L19" s="152"/>
+      <c r="M19" s="152"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="100" t="s">
+      <c r="A20" s="152" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="100"/>
-      <c r="I20" s="100"/>
-      <c r="J20" s="100"/>
-      <c r="K20" s="100"/>
-      <c r="L20" s="100"/>
-      <c r="M20" s="100"/>
+      <c r="B20" s="152"/>
+      <c r="C20" s="152"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="152"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="152"/>
+      <c r="J20" s="152"/>
+      <c r="K20" s="152"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="152"/>
     </row>
     <row r="23" spans="1:13" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
@@ -2651,20 +2678,20 @@
       <c r="A27" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="101" t="s">
+      <c r="B27" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="102"/>
-      <c r="D27" s="101" t="s">
+      <c r="C27" s="169"/>
+      <c r="D27" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="102"/>
+      <c r="E27" s="169"/>
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
-      <c r="H27" s="103" t="s">
+      <c r="H27" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="104"/>
+      <c r="I27" s="146"/>
       <c r="J27" s="86"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2827,20 +2854,20 @@
       <c r="A35" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="101" t="s">
+      <c r="B35" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="102"/>
-      <c r="D35" s="101" t="s">
+      <c r="C35" s="169"/>
+      <c r="D35" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="102"/>
+      <c r="E35" s="169"/>
       <c r="F35" s="40"/>
       <c r="G35" s="40"/>
-      <c r="H35" s="103" t="s">
+      <c r="H35" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="I35" s="104"/>
+      <c r="I35" s="146"/>
       <c r="J35" s="86"/>
       <c r="K35" s="24" t="s">
         <v>51</v>
@@ -2978,17 +3005,17 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" s="117" t="s">
+      <c r="A43" s="170" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="117"/>
-      <c r="C43" s="117"/>
-      <c r="D43" s="117"/>
-      <c r="E43" s="117"/>
-      <c r="F43" s="117"/>
-      <c r="G43" s="117"/>
-      <c r="H43" s="117"/>
-      <c r="I43" s="117"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="170"/>
+      <c r="D43" s="170"/>
+      <c r="E43" s="170"/>
+      <c r="F43" s="170"/>
+      <c r="G43" s="170"/>
+      <c r="H43" s="170"/>
+      <c r="I43" s="170"/>
       <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -3033,20 +3060,20 @@
       <c r="A46" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="101" t="s">
+      <c r="B46" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="102"/>
-      <c r="D46" s="101" t="s">
+      <c r="C46" s="169"/>
+      <c r="D46" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="102"/>
+      <c r="E46" s="169"/>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
-      <c r="H46" s="103" t="s">
+      <c r="H46" s="145" t="s">
         <v>58</v>
       </c>
-      <c r="I46" s="104"/>
+      <c r="I46" s="146"/>
       <c r="J46" s="86"/>
       <c r="N46" s="20"/>
       <c r="O46" s="20"/>
@@ -3222,20 +3249,20 @@
       <c r="A54" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B54" s="101" t="s">
+      <c r="B54" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="102"/>
-      <c r="D54" s="101" t="s">
+      <c r="C54" s="169"/>
+      <c r="D54" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="102"/>
+      <c r="E54" s="169"/>
       <c r="F54" s="40"/>
       <c r="G54" s="40"/>
-      <c r="H54" s="103" t="s">
+      <c r="H54" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="I54" s="104"/>
+      <c r="I54" s="146"/>
       <c r="J54" s="86"/>
       <c r="K54" s="24" t="s">
         <v>51</v>
@@ -3513,24 +3540,24 @@
       <c r="K66" s="68"/>
     </row>
     <row r="67" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="130" t="s">
+      <c r="A67" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="131" t="s">
+      <c r="B67" s="105" t="s">
         <v>85</v>
       </c>
-      <c r="C67" s="131"/>
-      <c r="D67" s="131"/>
-      <c r="E67" s="131"/>
-      <c r="F67" s="131"/>
-      <c r="G67" s="131"/>
-      <c r="H67" s="131"/>
-      <c r="I67" s="131"/>
-      <c r="J67" s="132"/>
-      <c r="K67" s="133"/>
+      <c r="C67" s="105"/>
+      <c r="D67" s="105"/>
+      <c r="E67" s="105"/>
+      <c r="F67" s="105"/>
+      <c r="G67" s="105"/>
+      <c r="H67" s="105"/>
+      <c r="I67" s="105"/>
+      <c r="J67" s="106"/>
+      <c r="K67" s="107"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A68" s="134" t="s">
+      <c r="A68" s="108" t="s">
         <v>62</v>
       </c>
       <c r="B68" s="66" t="s">
@@ -3560,7 +3587,7 @@
       <c r="J68" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="K68" s="135" t="s">
+      <c r="K68" s="109" t="s">
         <v>84</v>
       </c>
       <c r="L68" s="68"/>
@@ -3569,167 +3596,171 @@
       <c r="A69" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="B69" s="118" t="s">
+      <c r="B69" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="C69" s="119"/>
-      <c r="D69" s="118" t="s">
+      <c r="C69" s="144"/>
+      <c r="D69" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="E69" s="119"/>
-      <c r="F69" s="118" t="s">
+      <c r="E69" s="144"/>
+      <c r="F69" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="G69" s="119"/>
-      <c r="H69" s="103" t="s">
+      <c r="G69" s="144"/>
+      <c r="H69" s="145" t="s">
         <v>58</v>
       </c>
-      <c r="I69" s="104"/>
-      <c r="J69" s="124" t="s">
+      <c r="I69" s="146"/>
+      <c r="J69" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="K69" s="136"/>
+      <c r="K69" s="155"/>
       <c r="L69" s="68"/>
     </row>
     <row r="70" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="155">
+      <c r="A70" s="127">
         <v>0</v>
       </c>
-      <c r="B70" s="156">
+      <c r="B70" s="128">
         <v>20</v>
       </c>
-      <c r="C70" s="157">
+      <c r="C70" s="129">
         <v>54.03</v>
       </c>
-      <c r="D70" s="158">
+      <c r="D70" s="130">
         <v>239</v>
       </c>
-      <c r="E70" s="159">
+      <c r="E70" s="131">
         <v>605.79999999999995</v>
       </c>
-      <c r="F70" s="158">
+      <c r="F70" s="130">
         <v>142</v>
       </c>
-      <c r="G70" s="159">
+      <c r="G70" s="131">
         <v>3415</v>
       </c>
-      <c r="H70" s="158">
+      <c r="H70" s="130">
         <f>SUM(B70+D70+F70)</f>
         <v>401</v>
       </c>
-      <c r="I70" s="159">
+      <c r="I70" s="131">
         <f>SUM(C70+E70+G70)/3600</f>
         <v>1.1318972222222221</v>
       </c>
       <c r="J70" s="87">
         <v>137</v>
       </c>
-      <c r="K70" s="137" t="s">
+      <c r="K70" s="110" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A71" s="165">
+      <c r="A71" s="137">
         <v>3</v>
       </c>
-      <c r="B71" s="166">
+      <c r="B71" s="138">
         <v>11</v>
       </c>
-      <c r="C71" s="167">
+      <c r="C71" s="139">
         <v>133.80000000000001</v>
       </c>
-      <c r="D71" s="168">
+      <c r="D71" s="140">
         <v>368</v>
       </c>
-      <c r="E71" s="169">
+      <c r="E71" s="141">
         <v>1813</v>
       </c>
-      <c r="F71" s="168">
+      <c r="F71" s="140">
         <v>82</v>
       </c>
-      <c r="G71" s="169">
+      <c r="G71" s="141">
         <v>11701</v>
       </c>
       <c r="H71" s="66">
         <f>SUM(B71+D71+F71)</f>
         <v>461</v>
       </c>
-      <c r="I71" s="170">
+      <c r="I71" s="142">
         <f>SUM(C71+E71+G71)/3600</f>
         <v>3.7910555555555554</v>
       </c>
       <c r="J71" s="89">
         <v>1024</v>
       </c>
-      <c r="K71" s="135" t="s">
+      <c r="K71" s="109" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A72" s="69">
+      <c r="A72" s="48">
         <v>12</v>
       </c>
-      <c r="B72" s="97">
+      <c r="B72" s="50">
         <v>152</v>
       </c>
-      <c r="C72" s="71">
+      <c r="C72" s="51">
         <v>182.1</v>
       </c>
-      <c r="D72" s="72">
-        <v>490</v>
-      </c>
-      <c r="E72" s="98">
-        <v>1966</v>
-      </c>
-      <c r="F72" s="72"/>
-      <c r="G72" s="98"/>
+      <c r="D72" s="49">
+        <v>493</v>
+      </c>
+      <c r="E72" s="52">
+        <v>1928</v>
+      </c>
+      <c r="F72" s="96"/>
+      <c r="G72" s="172"/>
       <c r="H72" s="72">
         <f t="shared" ref="H72:H76" si="12">SUM(B72+D72+F72)</f>
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="I72" s="98">
         <f t="shared" ref="I72:I76" si="13">SUM(C72+E72+G72)/3600</f>
-        <v>0.59669444444444442</v>
+        <v>0.58613888888888888</v>
       </c>
       <c r="J72" s="89"/>
-      <c r="K72" s="135"/>
+      <c r="K72" s="109"/>
       <c r="O72" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A73" s="69">
+      <c r="A73" s="48">
         <v>27</v>
       </c>
-      <c r="B73" s="97">
+      <c r="B73" s="50">
         <v>24</v>
       </c>
-      <c r="C73" s="71">
+      <c r="C73" s="51">
         <v>102</v>
       </c>
-      <c r="D73" s="72">
+      <c r="D73" s="49">
         <v>307</v>
       </c>
-      <c r="E73" s="98">
+      <c r="E73" s="52">
         <v>1386</v>
       </c>
-      <c r="F73" s="72"/>
-      <c r="G73" s="98"/>
+      <c r="F73" s="49">
+        <v>20</v>
+      </c>
+      <c r="G73" s="52">
+        <v>9853</v>
+      </c>
       <c r="H73" s="72">
         <f>SUM(B73+D73+F73)</f>
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="I73" s="98">
         <f t="shared" si="13"/>
-        <v>0.41333333333333333</v>
+        <v>3.1502777777777777</v>
       </c>
       <c r="J73" s="89">
         <f>SUM(H71:H74)</f>
-        <v>1886</v>
-      </c>
-      <c r="K73" s="135">
+        <v>1923</v>
+      </c>
+      <c r="K73" s="109">
         <f>SUM(I71:I74)</f>
-        <v>5.4646388888888886</v>
+        <v>8.1154722222222233</v>
       </c>
       <c r="N73">
         <v>1</v>
@@ -3739,35 +3770,35 @@
       </c>
     </row>
     <row r="74" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="75">
+      <c r="A74" s="171">
         <v>47</v>
       </c>
-      <c r="B74" s="76">
+      <c r="B74" s="101">
         <v>75</v>
       </c>
-      <c r="C74" s="77">
+      <c r="C74" s="102">
         <v>155.80000000000001</v>
       </c>
-      <c r="D74" s="78">
-        <v>377</v>
-      </c>
-      <c r="E74" s="79">
-        <v>2233</v>
-      </c>
-      <c r="F74" s="78"/>
-      <c r="G74" s="79"/>
+      <c r="D74" s="59">
+        <v>391</v>
+      </c>
+      <c r="E74" s="126">
+        <v>1961</v>
+      </c>
+      <c r="F74" s="173"/>
+      <c r="G74" s="174"/>
       <c r="H74" s="78">
         <f>SUM(B74+D74+F74)</f>
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="I74" s="79">
         <f t="shared" si="13"/>
-        <v>0.66355555555555557</v>
+        <v>0.58800000000000008</v>
       </c>
       <c r="J74" s="89"/>
-      <c r="K74" s="135">
+      <c r="K74" s="109">
         <f>K73/4</f>
-        <v>1.3661597222222222</v>
+        <v>2.0288680555555558</v>
       </c>
       <c r="N74">
         <v>2</v>
@@ -3780,39 +3811,39 @@
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A75" s="160">
+      <c r="A75" s="132">
         <v>52</v>
       </c>
-      <c r="B75" s="161">
+      <c r="B75" s="133">
         <v>5</v>
       </c>
-      <c r="C75" s="162">
+      <c r="C75" s="134">
         <v>8.5749999999999993</v>
       </c>
-      <c r="D75" s="163">
+      <c r="D75" s="135">
         <v>0</v>
       </c>
-      <c r="E75" s="164">
+      <c r="E75" s="136">
         <v>117.4</v>
       </c>
-      <c r="F75" s="163">
+      <c r="F75" s="135">
         <v>0</v>
       </c>
-      <c r="G75" s="162">
+      <c r="G75" s="134">
         <v>76.59</v>
       </c>
-      <c r="H75" s="163">
+      <c r="H75" s="135">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="I75" s="164">
+      <c r="I75" s="136">
         <f t="shared" si="13"/>
         <v>5.6268055555555557E-2</v>
       </c>
-      <c r="J75" s="138">
+      <c r="J75" s="111">
         <v>52</v>
       </c>
-      <c r="K75" s="139" t="s">
+      <c r="K75" s="112" t="s">
         <v>87</v>
       </c>
       <c r="N75">
@@ -3823,76 +3854,76 @@
       </c>
     </row>
     <row r="76" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="140">
+      <c r="A76" s="113">
         <v>163</v>
       </c>
-      <c r="B76" s="125">
+      <c r="B76" s="101">
         <v>18</v>
       </c>
-      <c r="C76" s="126">
+      <c r="C76" s="102">
         <v>56.07</v>
       </c>
       <c r="D76" s="59">
         <v>240</v>
       </c>
-      <c r="E76" s="153">
+      <c r="E76" s="126">
         <v>936.5</v>
       </c>
       <c r="F76" s="59">
         <v>32</v>
       </c>
-      <c r="G76" s="153">
+      <c r="G76" s="126">
         <v>8232</v>
       </c>
       <c r="H76" s="59">
         <f t="shared" si="12"/>
         <v>290</v>
       </c>
-      <c r="I76" s="153">
+      <c r="I76" s="126">
         <f t="shared" si="13"/>
         <v>2.5623805555555554</v>
       </c>
       <c r="J76" s="87">
         <v>229</v>
       </c>
-      <c r="K76" s="137" t="s">
+      <c r="K76" s="110" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A77" s="141"/>
-      <c r="B77" s="142"/>
-      <c r="C77" s="142"/>
-      <c r="D77" s="142"/>
-      <c r="E77" s="142"/>
-      <c r="F77" s="154" t="s">
+      <c r="A77" s="114"/>
+      <c r="B77" s="115"/>
+      <c r="C77" s="115"/>
+      <c r="D77" s="115"/>
+      <c r="E77" s="115"/>
+      <c r="F77" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="G77" s="154"/>
-      <c r="H77" s="142"/>
-      <c r="I77" s="142"/>
-      <c r="J77" s="142"/>
-      <c r="K77" s="143"/>
+      <c r="G77" s="149"/>
+      <c r="H77" s="115"/>
+      <c r="I77" s="115"/>
+      <c r="J77" s="115"/>
+      <c r="K77" s="116"/>
       <c r="O77" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="141" t="s">
+      <c r="A78" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="B78" s="144" t="s">
+      <c r="B78" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="C78" s="142"/>
-      <c r="D78" s="142"/>
-      <c r="E78" s="142"/>
-      <c r="F78" s="144"/>
-      <c r="G78" s="142"/>
-      <c r="H78" s="142"/>
-      <c r="I78" s="142"/>
-      <c r="J78" s="142"/>
-      <c r="K78" s="145"/>
+      <c r="C78" s="115"/>
+      <c r="D78" s="115"/>
+      <c r="E78" s="115"/>
+      <c r="F78" s="117"/>
+      <c r="G78" s="115"/>
+      <c r="H78" s="115"/>
+      <c r="I78" s="115"/>
+      <c r="J78" s="115"/>
+      <c r="K78" s="118"/>
       <c r="O78" t="s">
         <v>69</v>
       </c>
@@ -3904,7 +3935,7 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A79" s="134" t="s">
+      <c r="A79" s="108" t="s">
         <v>62</v>
       </c>
       <c r="B79" s="66" t="s">
@@ -3922,7 +3953,7 @@
       <c r="F79" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="G79" s="128" t="s">
+      <c r="G79" s="103" t="s">
         <v>82</v>
       </c>
       <c r="H79" s="66" t="s">
@@ -3931,31 +3962,31 @@
       <c r="I79" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="J79" s="142"/>
-      <c r="K79" s="145"/>
+      <c r="J79" s="115"/>
+      <c r="K79" s="118"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="B80" s="118" t="s">
+      <c r="B80" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="C80" s="119"/>
-      <c r="D80" s="118" t="s">
+      <c r="C80" s="144"/>
+      <c r="D80" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="E80" s="119"/>
-      <c r="F80" s="118" t="s">
+      <c r="E80" s="144"/>
+      <c r="F80" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="G80" s="129"/>
-      <c r="H80" s="127" t="s">
+      <c r="G80" s="147"/>
+      <c r="H80" s="148" t="s">
         <v>58</v>
       </c>
-      <c r="I80" s="104"/>
-      <c r="J80" s="142"/>
-      <c r="K80" s="146"/>
+      <c r="I80" s="146"/>
+      <c r="J80" s="115"/>
+      <c r="K80" s="119"/>
       <c r="O80" t="s">
         <v>75</v>
       </c>
@@ -3993,7 +4024,7 @@
         <v>1930</v>
       </c>
       <c r="J81" s="89"/>
-      <c r="K81" s="143"/>
+      <c r="K81" s="116"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="95">
@@ -4022,9 +4053,9 @@
         <v>2148.1</v>
       </c>
       <c r="J82" s="89"/>
-      <c r="K82" s="145"/>
+      <c r="K82" s="118"/>
       <c r="L82" s="68"/>
-      <c r="O82" s="123" t="s">
+      <c r="O82" s="100" t="s">
         <v>79</v>
       </c>
       <c r="P82" t="s">
@@ -4058,11 +4089,11 @@
         <v>1488</v>
       </c>
       <c r="J83" s="89"/>
-      <c r="K83" s="145"/>
+      <c r="K83" s="118"/>
       <c r="L83" s="74"/>
     </row>
     <row r="84" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="147">
+      <c r="A84" s="120">
         <v>47</v>
       </c>
       <c r="B84" s="76">
@@ -4088,40 +4119,40 @@
         <v>2388.8000000000002</v>
       </c>
       <c r="J84" s="89"/>
-      <c r="K84" s="145"/>
+      <c r="K84" s="118"/>
       <c r="L84" s="74"/>
     </row>
     <row r="85" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="148"/>
-      <c r="B85" s="149"/>
-      <c r="C85" s="149"/>
-      <c r="D85" s="149"/>
-      <c r="E85" s="149"/>
-      <c r="F85" s="149"/>
-      <c r="G85" s="149"/>
-      <c r="H85" s="150">
+      <c r="A85" s="121"/>
+      <c r="B85" s="122"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
+      <c r="E85" s="122"/>
+      <c r="F85" s="122"/>
+      <c r="G85" s="122"/>
+      <c r="H85" s="123">
         <f>SUM(H81:H84)</f>
         <v>1807</v>
       </c>
-      <c r="I85" s="151">
+      <c r="I85" s="124">
         <v>1024</v>
       </c>
-      <c r="J85" s="149"/>
-      <c r="K85" s="152"/>
+      <c r="J85" s="122"/>
+      <c r="K85" s="125"/>
       <c r="L85" s="68"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A86" s="142"/>
-      <c r="B86" s="142"/>
-      <c r="C86" s="142"/>
-      <c r="D86" s="142"/>
-      <c r="E86" s="142"/>
-      <c r="F86" s="142"/>
-      <c r="G86" s="142"/>
+      <c r="A86" s="115"/>
+      <c r="B86" s="115"/>
+      <c r="C86" s="115"/>
+      <c r="D86" s="115"/>
+      <c r="E86" s="115"/>
+      <c r="F86" s="115"/>
+      <c r="G86" s="115"/>
       <c r="H86" s="89"/>
       <c r="I86" s="89"/>
-      <c r="J86" s="142"/>
-      <c r="K86" s="142"/>
+      <c r="J86" s="115"/>
+      <c r="K86" s="115"/>
       <c r="L86" s="68"/>
     </row>
     <row r="87" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -4174,20 +4205,20 @@
       <c r="A89" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B89" s="118" t="s">
+      <c r="B89" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="C89" s="119"/>
-      <c r="D89" s="118" t="s">
+      <c r="C89" s="144"/>
+      <c r="D89" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="E89" s="119"/>
+      <c r="E89" s="144"/>
       <c r="F89" s="85"/>
       <c r="G89" s="85"/>
-      <c r="H89" s="103" t="s">
+      <c r="H89" s="145" t="s">
         <v>58</v>
       </c>
-      <c r="I89" s="104"/>
+      <c r="I89" s="146"/>
       <c r="J89" s="86"/>
       <c r="K89" s="68"/>
       <c r="L89" s="68"/>
@@ -4354,20 +4385,20 @@
       <c r="A96" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B96" s="118" t="s">
+      <c r="B96" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="C96" s="119"/>
-      <c r="D96" s="118" t="s">
+      <c r="C96" s="144"/>
+      <c r="D96" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="E96" s="119"/>
+      <c r="E96" s="144"/>
       <c r="F96" s="85"/>
       <c r="G96" s="85"/>
-      <c r="H96" s="103" t="s">
+      <c r="H96" s="145" t="s">
         <v>58</v>
       </c>
-      <c r="I96" s="104"/>
+      <c r="I96" s="146"/>
       <c r="J96" s="86"/>
       <c r="K96" s="81" t="s">
         <v>51</v>
@@ -4585,49 +4616,24 @@
     </row>
     <row r="114" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B114" s="26"/>
-      <c r="C114" s="100" t="s">
+      <c r="C114" s="152" t="s">
         <v>38</v>
       </c>
-      <c r="D114" s="100"/>
-      <c r="E114" s="100"/>
-      <c r="F114" s="100"/>
-      <c r="G114" s="100"/>
-      <c r="H114" s="100"/>
-      <c r="I114" s="100" t="s">
+      <c r="D114" s="152"/>
+      <c r="E114" s="152"/>
+      <c r="F114" s="152"/>
+      <c r="G114" s="152"/>
+      <c r="H114" s="152"/>
+      <c r="I114" s="152" t="s">
         <v>39</v>
       </c>
-      <c r="J114" s="100"/>
-      <c r="K114" s="100"/>
-      <c r="L114" s="100"/>
-      <c r="M114" s="100"/>
+      <c r="J114" s="152"/>
+      <c r="K114" s="152"/>
+      <c r="L114" s="152"/>
+      <c r="M114" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A19:M19"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="K6:K8"/>
     <mergeCell ref="C114:H114"/>
     <mergeCell ref="I114:M114"/>
     <mergeCell ref="B27:C27"/>
@@ -4644,6 +4650,31 @@
     <mergeCell ref="H54:I54"/>
     <mergeCell ref="A43:I43"/>
     <mergeCell ref="B69:C69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="H69:I69"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>